<commit_message>
Update factsheets with text edits from COMM
</commit_message>
<xml_diff>
--- a/data/processed/national_overview.xlsx
+++ b/data/processed/national_overview.xlsx
@@ -388,8 +388,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>103475</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>103,475</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -419,7 +421,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,8 +465,10 @@
           <t>Alabama</t>
         </is>
       </c>
-      <c r="B2">
-        <v>1118</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1,118</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -493,27 +497,29 @@
           <t>Alaska</t>
         </is>
       </c>
-      <c r="B3">
-        <v>541</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>548</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$844,890,776</t>
+          <t>$848,313,307</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7.22%</t>
+          <t>7.18%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-27.98%</t>
+          <t>-28.55%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>78.74%</t>
+          <t>79.01%</t>
         </is>
       </c>
     </row>
@@ -523,8 +529,10 @@
           <t>Arizona</t>
         </is>
       </c>
-      <c r="B4">
-        <v>1446</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1,446</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -553,8 +561,10 @@
           <t>Arkansas</t>
         </is>
       </c>
-      <c r="B5">
-        <v>843</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>843</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -583,12 +593,14 @@
           <t>California</t>
         </is>
       </c>
-      <c r="B6">
-        <v>10509</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10,513</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$42,130,785,826</t>
+          <t>$42,132,825,415</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -603,7 +615,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>65.69%</t>
+          <t>65.68%</t>
         </is>
       </c>
     </row>
@@ -613,8 +625,10 @@
           <t>Colorado</t>
         </is>
       </c>
-      <c r="B7">
-        <v>2634</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2,634</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -643,8 +657,10 @@
           <t>Connecticut</t>
         </is>
       </c>
-      <c r="B8">
-        <v>1561</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1,561</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -673,8 +689,10 @@
           <t>Delaware</t>
         </is>
       </c>
-      <c r="B9">
-        <v>514</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>514</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -703,8 +721,10 @@
           <t>District of Columbia</t>
         </is>
       </c>
-      <c r="B10">
-        <v>1592</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1,592</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -733,12 +753,14 @@
           <t>Florida</t>
         </is>
       </c>
-      <c r="B11">
-        <v>3977</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3,981</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$12,417,392,975</t>
+          <t>$12,417,989,542</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -753,7 +775,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>69.85%</t>
+          <t>69.86%</t>
         </is>
       </c>
     </row>
@@ -763,8 +785,10 @@
           <t>Georgia</t>
         </is>
       </c>
-      <c r="B12">
-        <v>2130</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2,130</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -793,8 +817,10 @@
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="B13">
-        <v>630</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>630</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -823,8 +849,10 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B14">
-        <v>477</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>477</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -853,27 +881,29 @@
           <t>Illinois</t>
         </is>
       </c>
-      <c r="B15">
-        <v>3464</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>3,468</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$9,963,723,760</t>
+          <t>$9,986,549,815</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>8.19%</t>
+          <t>8.22%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-13.33%</t>
+          <t>-13.23%</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>67.32%</t>
+          <t>67.30%</t>
         </is>
       </c>
     </row>
@@ -883,8 +913,10 @@
           <t>Indiana</t>
         </is>
       </c>
-      <c r="B16">
-        <v>2051</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2,051</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -913,8 +945,10 @@
           <t>Iowa</t>
         </is>
       </c>
-      <c r="B17">
-        <v>1294</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1,294</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -943,8 +977,10 @@
           <t>Kansas</t>
         </is>
       </c>
-      <c r="B18">
-        <v>971</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>971</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -973,8 +1009,10 @@
           <t>Kentucky</t>
         </is>
       </c>
-      <c r="B19">
-        <v>1138</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1,138</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1003,8 +1041,10 @@
           <t>Louisiana</t>
         </is>
       </c>
-      <c r="B20">
-        <v>1214</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1,214</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1033,8 +1073,10 @@
           <t>Maine</t>
         </is>
       </c>
-      <c r="B21">
-        <v>875</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>875</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1063,8 +1105,10 @@
           <t>Maryland</t>
         </is>
       </c>
-      <c r="B22">
-        <v>2487</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2,487</t>
+        </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1093,17 +1137,19 @@
           <t>Massachusetts</t>
         </is>
       </c>
-      <c r="B23">
-        <v>3016</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>3,018</t>
+        </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$10,165,179,596</t>
+          <t>$10,165,747,853</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>11.76%</t>
+          <t>11.74%</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1113,7 +1159,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>60.31%</t>
+          <t>60.30%</t>
         </is>
       </c>
     </row>
@@ -1123,27 +1169,29 @@
           <t>Michigan</t>
         </is>
       </c>
-      <c r="B24">
-        <v>2471</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2,473</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$4,576,893,290</t>
+          <t>$4,577,112,023</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>8.99%</t>
+          <t>9.00%</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-10.27%</t>
+          <t>-10.23%</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>65.84%</t>
+          <t>65.79%</t>
         </is>
       </c>
     </row>
@@ -1153,8 +1201,10 @@
           <t>Minnesota</t>
         </is>
       </c>
-      <c r="B25">
-        <v>2849</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2,849</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1183,8 +1233,10 @@
           <t>Mississippi</t>
         </is>
       </c>
-      <c r="B26">
-        <v>545</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1213,8 +1265,10 @@
           <t>Missouri</t>
         </is>
       </c>
-      <c r="B27">
-        <v>1959</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1,959</t>
+        </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1243,8 +1297,10 @@
           <t>Montana</t>
         </is>
       </c>
-      <c r="B28">
-        <v>667</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>667</t>
+        </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1273,8 +1329,10 @@
           <t>Nebraska</t>
         </is>
       </c>
-      <c r="B29">
-        <v>769</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>769</t>
+        </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1303,8 +1361,10 @@
           <t>Nevada</t>
         </is>
       </c>
-      <c r="B30">
-        <v>503</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>503</t>
+        </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1333,8 +1393,10 @@
           <t>New Hampshire</t>
         </is>
       </c>
-      <c r="B31">
-        <v>663</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>663</t>
+        </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1363,8 +1425,10 @@
           <t>New Jersey</t>
         </is>
       </c>
-      <c r="B32">
-        <v>2532</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2,532</t>
+        </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1393,8 +1457,10 @@
           <t>New Mexico</t>
         </is>
       </c>
-      <c r="B33">
-        <v>772</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>772</t>
+        </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1423,12 +1489,14 @@
           <t>New York</t>
         </is>
       </c>
-      <c r="B34">
-        <v>8740</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>8,743</t>
+        </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>$29,720,189,788</t>
+          <t>$29,720,633,621</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1453,27 +1521,29 @@
           <t>North Carolina</t>
         </is>
       </c>
-      <c r="B35">
-        <v>3262</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>3,264</t>
+        </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$7,190,647,067</t>
+          <t>$7,190,690,326</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>9.28%</t>
+          <t>9.29%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-19.37%</t>
+          <t>-19.34%</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>69.59%</t>
+          <t>69.55%</t>
         </is>
       </c>
     </row>
@@ -1483,8 +1553,10 @@
           <t>North Dakota</t>
         </is>
       </c>
-      <c r="B36">
-        <v>444</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1513,8 +1585,10 @@
           <t>Ohio</t>
         </is>
       </c>
-      <c r="B37">
-        <v>4025</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>4,025</t>
+        </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1543,8 +1617,10 @@
           <t>Oklahoma</t>
         </is>
       </c>
-      <c r="B38">
-        <v>906</v>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>906</t>
+        </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1573,8 +1649,10 @@
           <t>Oregon</t>
         </is>
       </c>
-      <c r="B39">
-        <v>1961</v>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1,961</t>
+        </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1600,20 +1678,22 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Other U.S. Territories</t>
-        </is>
-      </c>
-      <c r="B40">
-        <v>298</v>
+          <t>Other US Jurisdictions/Unmapped</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>388</t>
+        </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>$599,019,752</t>
+          <t>$744,980,831</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>5.28%</t>
+          <t>5.89%</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1623,7 +1703,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>83.89%</t>
+          <t>82.22%</t>
         </is>
       </c>
     </row>
@@ -1633,8 +1713,10 @@
           <t>Pennsylvania</t>
         </is>
       </c>
-      <c r="B41">
-        <v>6175</v>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>6,175</t>
+        </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1663,8 +1745,10 @@
           <t>Rhode Island</t>
         </is>
       </c>
-      <c r="B42">
-        <v>547</v>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>547</t>
+        </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1693,8 +1777,10 @@
           <t>South Carolina</t>
         </is>
       </c>
-      <c r="B43">
-        <v>1290</v>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1,290</t>
+        </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1723,8 +1809,10 @@
           <t>South Dakota</t>
         </is>
       </c>
-      <c r="B44">
-        <v>459</v>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>459</t>
+        </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1753,8 +1841,10 @@
           <t>Tennessee</t>
         </is>
       </c>
-      <c r="B45">
-        <v>2030</v>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2,030</t>
+        </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1783,8 +1873,10 @@
           <t>Texas</t>
         </is>
       </c>
-      <c r="B46">
-        <v>4750</v>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>4,750</t>
+        </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1810,268 +1902,254 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Unmapped</t>
-        </is>
-      </c>
-      <c r="B47">
-        <v>121</v>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>718</t>
+        </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>$176,791,337</t>
+          <t>$1,665,786,876</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>8.64%</t>
+          <t>9.73%</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>-22.49%</t>
+          <t>-23.91%</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>72.73%</t>
+          <t>72.14%</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="B48">
-        <v>718</v>
+          <t>Vermont</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>721</t>
+        </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>$1,665,786,876</t>
+          <t>$610,463,403</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>9.73%</t>
+          <t>8.62%</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>-23.91%</t>
+          <t>-10.12%</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>72.14%</t>
+          <t>66.71%</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Vermont</t>
-        </is>
-      </c>
-      <c r="B49">
-        <v>721</v>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2,792</t>
+        </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>$610,463,403</t>
+          <t>$4,571,835,868</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>8.62%</t>
+          <t>10.66%</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>-10.12%</t>
+          <t>-9.96%</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>66.71%</t>
+          <t>64.29%</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Virginia</t>
-        </is>
-      </c>
-      <c r="B50">
-        <v>2792</v>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2,741</t>
+        </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>$4,571,835,868</t>
+          <t>$6,452,428,730</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>10.66%</t>
+          <t>10.77%</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>-9.96%</t>
+          <t>-10.62%</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>64.29%</t>
+          <t>66.00%</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Washington</t>
-        </is>
-      </c>
-      <c r="B51">
-        <v>2739</v>
+          <t>West Virginia</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>769</t>
+        </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>$6,451,808,289</t>
+          <t>$1,067,242,685</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>10.77%</t>
+          <t>9.05%</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>-10.59%</t>
+          <t>-27.48%</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>65.97%</t>
+          <t>75.81%</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>West Virginia</t>
-        </is>
-      </c>
-      <c r="B52">
-        <v>769</v>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2,155</t>
+        </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>$1,067,242,685</t>
+          <t>$3,131,962,290</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>9.05%</t>
+          <t>10.44%</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>-27.48%</t>
+          <t>-8.25%</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>75.81%</t>
+          <t>63.53%</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
-        </is>
-      </c>
-      <c r="B53">
-        <v>2154</v>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>362</t>
+        </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>$3,131,911,297</t>
+          <t>$261,596,078</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>10.44%</t>
+          <t>6.11%</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>-8.27%</t>
+          <t>-25.29%</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>63.56%</t>
+          <t>68.78%</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Wyoming</t>
-        </is>
-      </c>
-      <c r="B54">
-        <v>362</v>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>103,475</t>
+        </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>$261,596,078</t>
+          <t>$267,700,640,005</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>6.11%</t>
+          <t>9.05%</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>-25.29%</t>
+          <t>-12.83%</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
-        <is>
-          <t>68.78%</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B55">
-        <v>103475</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>$267,700,640,005</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>9.05%</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>-12.83%</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
         <is>
           <t>67.35%</t>
         </is>
@@ -2128,8 +2206,10 @@
           <t>Between $100K and $499K</t>
         </is>
       </c>
-      <c r="B2">
-        <v>31231</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>31,231</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2158,8 +2238,10 @@
           <t>Between $1M and $4.99M</t>
         </is>
       </c>
-      <c r="B3">
-        <v>28692</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>28,692</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2188,8 +2270,10 @@
           <t>Between $500K and $999K</t>
         </is>
       </c>
-      <c r="B4">
-        <v>16931</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>16,931</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2218,8 +2302,10 @@
           <t>Between $5M and $9.99M</t>
         </is>
       </c>
-      <c r="B5">
-        <v>7799</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>7,799</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2248,8 +2334,10 @@
           <t>Greater than $10M</t>
         </is>
       </c>
-      <c r="B6">
-        <v>13954</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>13,954</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2278,8 +2366,10 @@
           <t>Less than $100K</t>
         </is>
       </c>
-      <c r="B7">
-        <v>4868</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4,868</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2308,8 +2398,10 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="B8">
-        <v>103475</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>103,475</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2383,8 +2475,10 @@
           <t>Arts, Culture, and Humanities</t>
         </is>
       </c>
-      <c r="B2">
-        <v>9965</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9,965</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2413,8 +2507,10 @@
           <t>Education (Excluding Universities)</t>
         </is>
       </c>
-      <c r="B3">
-        <v>11982</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11,982</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2443,8 +2539,10 @@
           <t>Environment and Animals</t>
         </is>
       </c>
-      <c r="B4">
-        <v>4483</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4,483</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2473,8 +2571,10 @@
           <t>Health (Excluding Hospitals)</t>
         </is>
       </c>
-      <c r="B5">
-        <v>9428</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9,428</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2503,8 +2603,10 @@
           <t>Hospitals</t>
         </is>
       </c>
-      <c r="B6">
-        <v>1151</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1,151</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2533,8 +2635,10 @@
           <t>Human Services</t>
         </is>
       </c>
-      <c r="B7">
-        <v>32031</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>32,031</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2563,8 +2667,10 @@
           <t>International, Foreign Affairs</t>
         </is>
       </c>
-      <c r="B8">
-        <v>1230</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1,230</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2593,8 +2699,10 @@
           <t>Mutual/Membership Benefit</t>
         </is>
       </c>
-      <c r="B9">
-        <v>65</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2623,8 +2731,10 @@
           <t>Public, Societal Benefit</t>
         </is>
       </c>
-      <c r="B10">
-        <v>8292</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>8,292</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -2653,8 +2763,10 @@
           <t>Religion Related</t>
         </is>
       </c>
-      <c r="B11">
-        <v>2359</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2,359</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -2683,8 +2795,10 @@
           <t>Unclassified</t>
         </is>
       </c>
-      <c r="B12">
-        <v>21321</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21,321</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -2713,8 +2827,10 @@
           <t>Universities</t>
         </is>
       </c>
-      <c r="B13">
-        <v>1168</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1,168</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -2743,8 +2859,10 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="B14">
-        <v>103475</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>103,475</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
This commit accomplishes the following:
- Edit text according to COMM's revised edits found in this box note:
https://urbanorg.app.box.com/notes/1960559310379?s=s98mf6ihbgm7n9k90tavrbzy7fjsyio7
- Update the processed datastet to edit text for unmapped jurisdictions
- Remove the yellow shading in the factsheets for clarity
- Renames table columns based on COMM's updated column names
- Recreates all datasets used in factsheets based on Box notes
</commit_message>
<xml_diff>
--- a/data/processed/national_overview.xlsx
+++ b/data/processed/national_overview.xlsx
@@ -363,54 +363,54 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Share of 990 filers with government grants at risk</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Number of 990 filers with government grants</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Total government grants ($)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Operating surplus with government grants (%)</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Operating surplus without government grants (%)</t>
+          <t>Size of operating surplus with government grants</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Share of 990 filers with government grants at risk</t>
+          <t>Size of operating surplus without government grants</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>67.35%</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>103,475</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>$267,700,640,005</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>9.05%</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>-12.83%</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>67.35%</t>
         </is>
       </c>
     </row>
@@ -435,27 +435,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Share of 990 filers with government grants at risk</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Number of 990 filers with government grants</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Total government grants ($)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Operating surplus with government grants (%)</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Operating surplus without government grants (%)</t>
+          <t>Size of operating surplus with government grants</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Share of 990 filers with government grants at risk</t>
+          <t>Size of operating surplus without government grants</t>
         </is>
       </c>
     </row>
@@ -467,27 +467,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>67.35%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>103,475</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>$267,700,640,005</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>9.05%</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>-12.83%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>67.35%</t>
         </is>
       </c>
     </row>
@@ -499,27 +499,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>72.00%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>1,118</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>$1,944,864,228</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>7.87%</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>-21.45%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>72.00%</t>
         </is>
       </c>
     </row>
@@ -531,27 +531,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>79.01%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>548</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>$848,313,307</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>7.18%</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>-28.55%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>79.01%</t>
         </is>
       </c>
     </row>
@@ -563,27 +563,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>65.98%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>1,446</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>$3,710,995,891</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>8.70%</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>-12.71%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>65.98%</t>
         </is>
       </c>
     </row>
@@ -595,27 +595,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>75.21%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>843</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>$1,497,047,399</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>7.13%</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>-20.99%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>75.21%</t>
         </is>
       </c>
     </row>
@@ -627,27 +627,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>65.68%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>10,513</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>$42,132,825,415</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>9.03%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>-13.04%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>65.68%</t>
         </is>
       </c>
     </row>
@@ -659,27 +659,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>59.83%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>2,634</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>$3,482,686,129</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>11.50%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>-6.54%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>59.83%</t>
         </is>
       </c>
     </row>
@@ -691,27 +691,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>71.11%</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>1,561</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>$3,847,910,957</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>7.14%</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>-16.67%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>71.11%</t>
         </is>
       </c>
     </row>
@@ -723,27 +723,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>73.54%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>514</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>$1,256,309,593</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>9.93%</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>-26.82%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>73.54%</t>
         </is>
       </c>
     </row>
@@ -755,27 +755,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>62.94%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>1,592</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>$18,688,408,098</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>9.72%</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>-9.87%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>62.94%</t>
         </is>
       </c>
     </row>
@@ -787,27 +787,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>69.86%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>3,981</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>$12,417,989,542</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>7.10%</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>-16.26%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>69.86%</t>
         </is>
       </c>
     </row>
@@ -819,27 +819,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>66.43%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>2,130</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>$5,229,883,749</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>9.35%</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>-11.79%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>66.43%</t>
         </is>
       </c>
     </row>
@@ -851,27 +851,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>70.00%</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>630</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>$1,081,113,515</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>8.92%</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>-17.37%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>70.00%</t>
         </is>
       </c>
     </row>
@@ -883,27 +883,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>62.05%</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>477</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>$643,142,727</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>12.56%</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>-11.31%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>62.05%</t>
         </is>
       </c>
     </row>
@@ -915,27 +915,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>67.30%</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>3,468</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>$9,986,549,815</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>8.22%</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>-13.23%</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>67.30%</t>
         </is>
       </c>
     </row>
@@ -947,27 +947,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>65.24%</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>2,051</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>$3,305,071,391</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>10.03%</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>-11.39%</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>65.24%</t>
         </is>
       </c>
     </row>
@@ -979,27 +979,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>62.36%</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>1,294</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>$1,252,625,535</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>10.37%</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>-5.73%</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>62.36%</t>
         </is>
       </c>
     </row>
@@ -1011,27 +1011,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>70.13%</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>971</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>$1,044,083,084</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>8.02%</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>-11.92%</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>70.13%</t>
         </is>
       </c>
     </row>
@@ -1043,27 +1043,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>65.64%</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>1,138</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>$2,425,907,719</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>9.25%</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>-10.73%</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>65.64%</t>
         </is>
       </c>
     </row>
@@ -1075,27 +1075,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>72.08%</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>1,214</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>$2,869,770,671</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>7.97%</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>-27.48%</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>72.08%</t>
         </is>
       </c>
     </row>
@@ -1107,27 +1107,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>60.34%</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>875</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>$1,125,149,145</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>11.09%</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>-7.21%</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>60.34%</t>
         </is>
       </c>
     </row>
@@ -1139,27 +1139,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>69.08%</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>2,487</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>$6,127,216,573</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>8.58%</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>-15.15%</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>69.08%</t>
         </is>
       </c>
     </row>
@@ -1171,27 +1171,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>60.30%</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>3,018</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>$10,165,747,853</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>11.74%</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>-5.38%</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>60.30%</t>
         </is>
       </c>
     </row>
@@ -1203,27 +1203,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>65.79%</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>2,473</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>$4,577,112,023</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>9.00%</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>-10.23%</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>65.79%</t>
         </is>
       </c>
     </row>
@@ -1235,27 +1235,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>68.66%</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>2,849</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>$4,691,495,380</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>8.08%</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>-11.96%</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>68.66%</t>
         </is>
       </c>
     </row>
@@ -1267,27 +1267,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>74.13%</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>545</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>$855,145,071</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>6.46%</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>-26.56%</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>74.13%</t>
         </is>
       </c>
     </row>
@@ -1299,27 +1299,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>68.25%</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>1,959</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>$3,985,106,420</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>7.82%</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>-12.22%</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>68.25%</t>
         </is>
       </c>
     </row>
@@ -1331,27 +1331,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>63.72%</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>667</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>$680,827,015</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>9.74%</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>-10.06%</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>63.72%</t>
         </is>
       </c>
     </row>
@@ -1363,27 +1363,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>65.28%</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>769</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>$986,876,099</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>7.78%</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>-11.28%</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>65.28%</t>
         </is>
       </c>
     </row>
@@ -1395,27 +1395,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>73.76%</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>503</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>$1,252,051,703</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>7.25%</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>-23.82%</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>73.76%</t>
         </is>
       </c>
     </row>
@@ -1427,27 +1427,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>62.90%</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>663</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>$1,133,383,584</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>10.55%</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>-7.39%</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>62.90%</t>
         </is>
       </c>
     </row>
@@ -1459,27 +1459,27 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>69.47%</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>2,532</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>$5,748,555,291</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>8.71%</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>-15.65%</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>69.47%</t>
         </is>
       </c>
     </row>
@@ -1491,27 +1491,27 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>70.47%</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>772</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>$943,744,428</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>10.15%</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>-16.09%</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>70.47%</t>
         </is>
       </c>
     </row>
@@ -1523,27 +1523,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>69.53%</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>8,743</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>$29,720,633,621</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>8.36%</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>-12.97%</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>69.53%</t>
         </is>
       </c>
     </row>
@@ -1555,27 +1555,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>69.55%</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>3,264</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>$7,190,690,326</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>9.29%</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>-19.34%</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>69.55%</t>
         </is>
       </c>
     </row>
@@ -1587,27 +1587,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>61.49%</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>444</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>$455,735,134</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>9.73%</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>-6.94%</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>61.49%</t>
         </is>
       </c>
     </row>
@@ -1619,27 +1619,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>71.45%</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>4,025</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>$7,999,510,499</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>7.17%</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>-17.50%</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>71.45%</t>
         </is>
       </c>
     </row>
@@ -1651,27 +1651,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>72.63%</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>906</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>$1,608,045,127</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>6.01%</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>-20.07%</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>72.63%</t>
         </is>
       </c>
     </row>
@@ -1683,59 +1683,59 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>67.31%</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>1,961</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>$3,508,813,229</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>11.60%</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>-13.87%</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>67.31%</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Other US Jurisdictions/Unmapped</t>
+          <t>Other/unmapped jurisdictions</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>82.22%</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>388</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>$744,980,831</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>5.89%</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>-30.53%</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>82.22%</t>
         </is>
       </c>
     </row>
@@ -1747,27 +1747,27 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>66.87%</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>6,175</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>$13,203,162,114</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>9.69%</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>-11.29%</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>66.87%</t>
         </is>
       </c>
     </row>
@@ -1779,27 +1779,27 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>66.00%</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>547</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>$1,009,094,930</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>9.60%</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>-11.45%</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>66.00%</t>
         </is>
       </c>
     </row>
@@ -1811,27 +1811,27 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>70.54%</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>1,290</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>$2,159,545,458</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>9.53%</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>-19.89%</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>70.54%</t>
         </is>
       </c>
     </row>
@@ -1843,27 +1843,27 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>59.69%</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>459</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>$812,178,184</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>11.76%</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>-5.43%</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>59.69%</t>
         </is>
       </c>
     </row>
@@ -1875,27 +1875,27 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>69.16%</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>2,030</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>$3,759,003,111</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>8.54%</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>-16.99%</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>69.16%</t>
         </is>
       </c>
     </row>
@@ -1907,27 +1907,27 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>65.05%</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>4,750</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>$17,830,022,161</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>9.58%</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>-10.73%</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>65.05%</t>
         </is>
       </c>
     </row>
@@ -1939,27 +1939,27 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>72.14%</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>718</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>$1,665,786,876</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>9.73%</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>-23.91%</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>72.14%</t>
         </is>
       </c>
     </row>
@@ -1971,27 +1971,27 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>66.71%</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>721</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>$610,463,403</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>8.62%</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>-10.12%</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>66.71%</t>
         </is>
       </c>
     </row>
@@ -2003,27 +2003,27 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>64.29%</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>2,792</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>$4,571,835,868</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>10.66%</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>-9.96%</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>64.29%</t>
         </is>
       </c>
     </row>
@@ -2035,27 +2035,27 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>66.00%</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>2,741</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>$6,452,428,730</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>10.77%</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>-10.62%</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>66.00%</t>
         </is>
       </c>
     </row>
@@ -2067,27 +2067,27 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>75.81%</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>769</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>$1,067,242,685</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>9.05%</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>-27.48%</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>75.81%</t>
         </is>
       </c>
     </row>
@@ -2099,27 +2099,27 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>63.53%</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>2,155</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>$3,131,962,290</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>10.44%</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>-8.25%</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>63.53%</t>
         </is>
       </c>
     </row>
@@ -2131,27 +2131,27 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>68.78%</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>362</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>$261,596,078</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>6.11%</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>-25.29%</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>68.78%</t>
         </is>
       </c>
     </row>
@@ -2176,187 +2176,187 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Share of 990 filers with government grants at risk</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Number of 990 filers with government grants</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Total government grants ($)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Operating surplus with government grants (%)</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Operating surplus without government grants (%)</t>
+          <t>Size of operating surplus with government grants</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Share of 990 filers with government grants at risk</t>
+          <t>Size of operating surplus without government grants</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>$100K to $499K</t>
+          <t>Between $100K and $499K</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>66.49%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>31,231</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>$3,620,918,180</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>11.14%</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>-14.42%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>66.49%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>$10M or more</t>
+          <t>Between $1M and $4.99M</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>13,954</t>
+          <t>68.40%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$209,956,876,844</t>
+          <t>28,692</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5.32%</t>
+          <t>$26,093,002,762</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-8.12%</t>
+          <t>9.08%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>67.60%</t>
+          <t>-13.78%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>$1M to $4.9M</t>
+          <t>Between $500K and $999K</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>28,692</t>
+          <t>67.55%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$26,093,002,762</t>
+          <t>16,931</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9.08%</t>
+          <t>$5,952,877,808</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-13.78%</t>
+          <t>9.65%</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>68.40%</t>
+          <t>-13.87%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>$500K to $999K</t>
+          <t>Between $5M and $9.99M</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16,931</t>
+          <t>70.71%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$5,952,877,808</t>
+          <t>7,799</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9.65%</t>
+          <t>$21,730,929,396</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-13.87%</t>
+          <t>7.20%</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>67.55%</t>
+          <t>-14.47%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>$5M to $9.9M</t>
+          <t>Greater than $10M</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7,799</t>
+          <t>67.60%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$21,730,929,396</t>
+          <t>13,954</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>7.20%</t>
+          <t>$209,956,876,844</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-14.47%</t>
+          <t>5.32%</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>70.71%</t>
+          <t>-8.12%</t>
         </is>
       </c>
     </row>
@@ -2368,27 +2368,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>59.86%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>4,868</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>$346,035,015</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>26.98%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>-10.72%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>59.86%</t>
         </is>
       </c>
     </row>
@@ -2400,27 +2400,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>67.35%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>103,475</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>$267,700,640,005</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>9.05%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>-12.83%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>67.35%</t>
         </is>
       </c>
     </row>
@@ -2445,155 +2445,155 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Share of 990 filers with government grants at risk</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Number of 990 filers with government grants</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Total government grants ($)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Operating surplus with government grants (%)</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Operating surplus without government grants (%)</t>
+          <t>Size of operating surplus with government grants</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Share of 990 filers with government grants at risk</t>
+          <t>Size of operating surplus without government grants</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arts, culture, and humanities</t>
+          <t>Arts, Culture, and Humanities</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>63.84%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>9,965</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>$6,574,150,795</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>13.88%</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>-9.42%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>63.84%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Education</t>
+          <t>Education (Excluding Universities)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>68.38%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>11,982</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>$37,388,011,297</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>8.78%</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>-13.49%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>68.38%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Environment and animals</t>
+          <t>Environment and Animals</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>50.95%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>4,483</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>$5,323,561,781</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>16.04%</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>-0.62%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>50.95%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Health</t>
+          <t>Health (Excluding Hospitals)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>69.81%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>9,428</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>$27,572,239,818</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>7.86%</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>-13.80%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>69.81%</t>
         </is>
       </c>
     </row>
@@ -2605,251 +2605,251 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>53.08%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>1,151</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>$9,090,157,551</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>5.62%</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>-0.99%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>53.08%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Human services</t>
+          <t>Human Services</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>70.50%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>32,031</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>$55,608,422,734</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>8.13%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>-18.16%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>70.50%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>International, foreign affairs</t>
+          <t>International, Foreign Affairs</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>56.99%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>1,230</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>$19,366,190,049</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>8.37%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>-4.17%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>56.99%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Public, societal benefit</t>
+          <t>Mutual/Membership Benefit</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8,292</t>
+          <t>66.15%</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$16,815,762,865</t>
+          <t>65</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10.39%</t>
+          <t>$27,279,912</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-16.66%</t>
+          <t>6.87%</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>66.71%</t>
+          <t>-25.91%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Religion-related</t>
+          <t>Public, Societal Benefit</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2,359</t>
+          <t>66.71%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$1,531,436,171</t>
+          <t>8,292</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12.16%</t>
+          <t>$16,815,762,865</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-0.88%</t>
+          <t>10.39%</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>51.89%</t>
+          <t>-16.66%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mutual/membership benefit</t>
+          <t>Religion Related</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>51.89%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$27,279,912</t>
+          <t>2,359</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6.87%</t>
+          <t>$1,531,436,171</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-25.91%</t>
+          <t>12.16%</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>66.15%</t>
+          <t>-0.88%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Universities</t>
+          <t>Unclassified</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1,168</t>
+          <t>69.78%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$26,851,897,779</t>
+          <t>21,321</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5.94%</t>
+          <t>$61,551,529,253</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-2.81%</t>
+          <t>8.03%</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>59.67%</t>
+          <t>-14.17%</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Unclassified</t>
+          <t>Universities</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21,321</t>
+          <t>59.67%</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$61,551,529,253</t>
+          <t>1,168</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8.03%</t>
+          <t>$26,851,897,779</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-14.17%</t>
+          <t>5.94%</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>69.78%</t>
+          <t>-2.81%</t>
         </is>
       </c>
     </row>
@@ -2861,27 +2861,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>67.35%</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>103,475</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>$267,700,640,005</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>9.05%</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>-12.83%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>67.35%</t>
         </is>
       </c>
     </row>

</xml_diff>